<commit_message>
change in overview sheet
</commit_message>
<xml_diff>
--- a/CP_proposal_power.xlsx
+++ b/CP_proposal_power.xlsx
@@ -501,7 +501,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -731,7 +731,7 @@
         <v>250</v>
       </c>
       <c r="I6" s="1">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="J6" s="5">
         <v>0.85199999999999998</v>

</xml_diff>